<commit_message>
tm final push +timestemp+date
</commit_message>
<xml_diff>
--- a/Optimezed version (beta)/test-gui/Time_measurement.xlsx
+++ b/Optimezed version (beta)/test-gui/Time_measurement.xlsx
@@ -4,50 +4,26 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <i val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -67,39 +43,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -456,72 +409,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
-  <cols>
-    <col width="10.36" customWidth="1" style="2" min="2" max="2"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="18.65" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>FUNCAO</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>TIME</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="13.8" customHeight="1" s="3">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>fantinato</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>8.344650268554688e-06</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9.298324584960938e-06</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>fantinato</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8.58306884765625e-06</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>fantinato melhor professor da each</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7.390975952148438e-06</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7.867813110351562e-06</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>fundos fundos fundos</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fundos fundos fundos</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>fundos fundos fundos</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>socorro</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4.76837158203125e-07</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>